<commit_message>
conti convento_workinprogress_almeno una entrata ed uscita
</commit_message>
<xml_diff>
--- a/conti_styled.xlsx
+++ b/conti_styled.xlsx
@@ -1162,19 +1162,19 @@
       <c r="B7" s="3" t="inlineStr"/>
       <c r="C7" s="3" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>698.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="n"/>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>Congrua</t>
+          <t>vuoto</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>698.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1182,11 +1182,11 @@
       <c r="B9" s="5" t="n"/>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>fra Giacomo</t>
+          <t>vuoto</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>698.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">

</xml_diff>